<commit_message>
Adding Zone Chart and option for KY Warehouses.
</commit_message>
<xml_diff>
--- a/TCG zone chart.xlsx
+++ b/TCG zone chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28217"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnologyDataServic\OneDrive - TCG3PL\Documents\Shipping Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnologyDataServic\OneDrive - TCG3PL\Documents\Shipping Tool\shipping_tool\NewGit\Shipping_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0317C757-A2CD-4768-8DBD-31B7D234213F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407CCFB1-FB12-4664-85E7-93D1E28D4F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="660" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{015FC8F6-AD59-4186-9588-7245133B6A03}"/>
   </bookViews>
@@ -25906,7 +25906,7 @@
   <dimension ref="A1:B907"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B907"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33176,6 +33176,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="49edbf36-c260-45c3-b495-bfb0584920cb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="95637587-5a6f-4f06-9a15-fdcb586f69c5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005D78D1FB4B9B5244B0B9838004E35D53" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a98489c6b9cceec948ea623c5359d439">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49edbf36-c260-45c3-b495-bfb0584920cb" xmlns:ns3="95637587-5a6f-4f06-9a15-fdcb586f69c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b1843906fec0a56ed78218964cc18b0" ns2:_="" ns3:_="">
     <xsd:import namespace="49edbf36-c260-45c3-b495-bfb0584920cb"/>
@@ -33384,27 +33404,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB28FB14-7C93-4AED-9239-CE7DE0690C78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="49edbf36-c260-45c3-b495-bfb0584920cb"/>
+    <ds:schemaRef ds:uri="95637587-5a6f-4f06-9a15-fdcb586f69c5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="49edbf36-c260-45c3-b495-bfb0584920cb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="95637587-5a6f-4f06-9a15-fdcb586f69c5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{327949D4-39DF-4606-9C78-9759AE1432FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{048C3800-15E2-4DE0-9780-A2B9757833A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33421,23 +33440,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{327949D4-39DF-4606-9C78-9759AE1432FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB28FB14-7C93-4AED-9239-CE7DE0690C78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="49edbf36-c260-45c3-b495-bfb0584920cb"/>
-    <ds:schemaRef ds:uri="95637587-5a6f-4f06-9a15-fdcb586f69c5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>